<commit_message>
fix multiple delivery items
</commit_message>
<xml_diff>
--- a/app/webroot/img/invoice_multiple.xlsx
+++ b/app/webroot/img/invoice_multiple.xlsx
@@ -296,110 +296,110 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +735,8 @@
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -761,82 +761,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="6.75" customHeight="1">
-      <c r="A1" s="62"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="5.25" customHeight="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="1:16" ht="5.25" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="1:16" ht="6.75" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
     </row>
     <row r="5" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A6" s="9"/>
@@ -848,9 +848,9 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="21" customHeight="1">
@@ -860,50 +860,50 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="29"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
@@ -911,228 +911,228 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A11" s="70"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
     </row>
     <row r="12" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="11"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="48"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="11"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
     </row>
     <row r="14" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="11"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
     </row>
     <row r="15" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="11"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
     </row>
     <row r="16" spans="1:16" ht="22.5" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
     </row>
     <row r="17" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
     </row>
     <row r="18" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
     </row>
     <row r="19" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
     </row>
     <row r="20" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A20" s="55"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
     </row>
     <row r="21" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
     </row>
     <row r="22" spans="1:17" ht="24" customHeight="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
     </row>
     <row r="23" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
     </row>
     <row r="24" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
     </row>
     <row r="25" spans="1:17" ht="27.75" customHeight="1">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="18" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
@@ -1158,15 +1158,15 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
@@ -1183,8 +1183,8 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
       <c r="M29" s="18"/>
       <c r="N29" s="25" t="s">
         <v>0</v>
@@ -1201,8 +1201,8 @@
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
       <c r="M30" s="18"/>
       <c r="N30" s="25" t="s">
         <v>1</v>
@@ -1219,8 +1219,8 @@
       <c r="H31" s="36"/>
       <c r="I31" s="36"/>
       <c r="J31" s="32"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
       <c r="M31" s="32"/>
       <c r="N31" s="38" t="s">
         <v>2</v>
@@ -1230,36 +1230,36 @@
       <c r="Q31" s="20"/>
     </row>
     <row r="32" spans="1:17" ht="24.75" customHeight="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
       <c r="J32" s="12"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
       <c r="M32" s="18"/>
       <c r="N32" s="26">
         <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
       <c r="J33" s="12"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
       <c r="M33" s="18"/>
       <c r="N33" s="25" t="s">
         <v>3</v>
@@ -1267,15 +1267,15 @@
       <c r="O33" s="5"/>
     </row>
     <row r="34" spans="1:15" ht="18" customHeight="1">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
       <c r="J34" s="12"/>
       <c r="L34" s="20"/>
       <c r="M34" s="18"/>
@@ -1295,41 +1295,41 @@
       <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:15" ht="21" customHeight="1">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
       <c r="J36" s="12"/>
       <c r="L36" s="20"/>
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:15" ht="9" customHeight="1">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
     </row>
     <row r="38" spans="1:15" s="6" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="31" t="s">
         <v>5</v>
       </c>
@@ -1337,50 +1337,50 @@
       <c r="G38" s="21"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
     </row>
     <row r="39" spans="1:15" ht="18" customHeight="1">
-      <c r="A39" s="50"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
+      <c r="A39" s="68"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
     </row>
     <row r="40" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A40" s="50"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="50"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="68"/>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
     </row>
     <row r="41" spans="1:15" ht="18" customHeight="1">
-      <c r="A41" s="50"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="22"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
       <c r="I41" s="22"/>
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
@@ -1393,89 +1393,38 @@
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="68"/>
+      <c r="J42" s="69"/>
+      <c r="K42" s="69"/>
+      <c r="L42" s="69"/>
+      <c r="M42" s="69"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="115">
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="K31:L31"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
@@ -1500,26 +1449,77 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="K29:L29"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0" right="0.19685039370078999" top="0.59055118110236005" bottom="0.43307086614173002" header="0.51181102362205" footer="0.47244094488188998"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix invoice dr number and add vatable sale
</commit_message>
<xml_diff>
--- a/app/webroot/img/invoice_multiple.xlsx
+++ b/app/webroot/img/invoice_multiple.xlsx
@@ -14,6 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$M$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -237,9 +238,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -299,66 +297,66 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +736,8 @@
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19:M19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -761,82 +762,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="6.75" customHeight="1">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="5.25" customHeight="1">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:16" ht="5.25" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:16" ht="6.75" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A6" s="9"/>
@@ -848,291 +849,287 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
     </row>
     <row r="12" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="47"/>
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
     </row>
     <row r="14" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:16" ht="22.5" customHeight="1">
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
     </row>
     <row r="16" spans="1:16" ht="22.5" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="17" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
     </row>
     <row r="18" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
     </row>
     <row r="19" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
       <c r="K19" s="47"/>
       <c r="L19" s="47"/>
       <c r="M19" s="47"/>
     </row>
     <row r="20" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
     </row>
     <row r="21" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
     </row>
     <row r="22" spans="1:17" ht="24" customHeight="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
     </row>
     <row r="23" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
     </row>
     <row r="24" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="67"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
     </row>
     <row r="25" spans="1:17" ht="27.75" customHeight="1">
-      <c r="A25" s="64"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="18" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
@@ -1145,9 +1142,9 @@
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
@@ -1158,253 +1155,253 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
-      <c r="M28" s="18"/>
+      <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="25" t="s">
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="25" t="s">
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="40" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="38" t="s">
+    <row r="31" spans="1:17" s="39" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="20"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="19"/>
     </row>
     <row r="32" spans="1:17" ht="24.75" customHeight="1">
-      <c r="A32" s="60"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
       <c r="J32" s="12"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="26">
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="25">
         <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A33" s="60"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
       <c r="J33" s="12"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="25" t="s">
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O33" s="5"/>
     </row>
     <row r="34" spans="1:15" ht="18" customHeight="1">
-      <c r="A34" s="60"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
       <c r="J34" s="12"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="18"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="17"/>
     </row>
     <row r="35" spans="1:15" ht="18" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="32"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="18"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="31"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36" spans="1:15" ht="21" customHeight="1">
-      <c r="A36" s="60"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
+      <c r="A36" s="54"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
       <c r="J36" s="12"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="18"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="17"/>
     </row>
     <row r="37" spans="1:15" ht="9" customHeight="1">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
+      <c r="A37" s="54"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
     </row>
     <row r="38" spans="1:15" s="6" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A38" s="70" t="s">
+      <c r="A38" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="31" t="s">
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="21"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="71"/>
-      <c r="K38" s="71"/>
-      <c r="L38" s="71"/>
-      <c r="M38" s="71"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
     </row>
     <row r="39" spans="1:15" ht="18" customHeight="1">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
-      <c r="L39" s="68"/>
-      <c r="M39" s="68"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
     </row>
     <row r="40" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A40" s="68"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="68"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
     </row>
     <row r="41" spans="1:15" ht="18" customHeight="1">
-      <c r="A41" s="68"/>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
+      <c r="A41" s="67"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
     </row>
     <row r="42" spans="1:15" ht="23.25" customHeight="1">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="68"/>
+      <c r="K42" s="68"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="68"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="115">
+  <mergeCells count="112">
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="G36:I36"/>
     <mergeCell ref="K33:L33"/>
@@ -1425,6 +1422,7 @@
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="K31:L31"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
@@ -1463,26 +1461,23 @@
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="K23:M23"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="K20:M20"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="K19:M19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M3"/>
     <mergeCell ref="A4:M4"/>
@@ -1511,15 +1506,14 @@
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:M16"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <pageMargins left="0" right="0.19685039370078999" top="0.59055118110236005" bottom="0.43307086614173002" header="0.51181102362205" footer="0.47244094488188998"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>